<commit_message>
Worked on my search some
</commit_message>
<xml_diff>
--- a/data/ospree_searchers/baskinsearches_emw.xlsx
+++ b/data/ospree_searchers/baskinsearches_emw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/projects/egret/data/ospree_searchers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B183A4C8-9805-F94B-B793-61D9DC0335DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B374440-9152-1849-A523-0B16073451C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1980" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{889A57AF-BF39-5D40-9210-6ED7C554C77F}"/>
+    <workbookView xWindow="11740" yWindow="5640" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{889A57AF-BF39-5D40-9210-6ED7C554C77F}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="69">
   <si>
     <t>genus</t>
   </si>
@@ -164,9 +164,6 @@
     <t>not sure</t>
   </si>
   <si>
-    <t xml:space="preserve"> it's in Chinese and it does not have our Viburnum species as best I can tell</t>
-  </si>
-  <si>
     <t>Gill &amp; Pogge, 1974</t>
   </si>
   <si>
@@ -210,6 +207,42 @@
   </si>
   <si>
     <t>many likely</t>
+  </si>
+  <si>
+    <t>Tilia</t>
+  </si>
+  <si>
+    <t>Rhododendron</t>
+  </si>
+  <si>
+    <t>Tiwari &amp; Chauhan, 2007</t>
+  </si>
+  <si>
+    <t>it's in Chinese and it does not have our Viburnum species as best I can tell … but has many of our genera (shows up again for Rhododendron and Syringa)  … should we scrape?</t>
+  </si>
+  <si>
+    <t>Syringa</t>
+  </si>
+  <si>
+    <t>generally not much in B2</t>
+  </si>
+  <si>
+    <t>yes (range)</t>
+  </si>
+  <si>
+    <t>Seems good (book Dan ordered -- what does Dan think?)</t>
+  </si>
+  <si>
+    <t>waiting on most refs stil from HU Scan &amp; Deliver … Did not write them out yet.</t>
+  </si>
+  <si>
+    <t>Google Scholar</t>
+  </si>
+  <si>
+    <t>Khudonogova_2019</t>
+  </si>
+  <si>
+    <t>they did different treatments depending on what they thought the plant dormancy type was</t>
   </si>
 </sst>
 </file>
@@ -716,10 +749,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12744717-5B93-A544-A605-382F84106D6C}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,7 +876,7 @@
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
@@ -864,8 +897,8 @@
       <c r="J4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
-        <v>42</v>
+      <c r="K4" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -879,13 +912,13 @@
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -896,16 +929,16 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -919,7 +952,7 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
@@ -937,10 +970,10 @@
         <v>33</v>
       </c>
       <c r="J7" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" t="s">
         <v>48</v>
-      </c>
-      <c r="K7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -954,13 +987,13 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -974,13 +1007,25 @@
         <v>28</v>
       </c>
       <c r="D9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+      <c r="G9" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" t="s">
+        <v>63</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -994,13 +1039,98 @@
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
         <v>35</v>
       </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>